<commit_message>
Timing and code optimizations, Execute (work in progress)
git-svn-id: https://svn.media.mit.edu/r/biomech-ee/Code/flexsea_1_0@450 ca98db78-25f0-4961-890e-003d10304561
</commit_message>
<xml_diff>
--- a/execute/ref/timing.xlsx
+++ b/execute/ref/timing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Time (µs)</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Cycle 1/4:</t>
+  </si>
+  <si>
+    <t>One of the 3 fcts</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="BE37" sqref="BE37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,14 +1335,11 @@
       <c r="CY14" s="12"/>
     </row>
     <row r="15" spans="1:103" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -1643,14 +1643,11 @@
       </c>
     </row>
     <row r="16" spans="1:103" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>250</v>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="7"/>
@@ -1674,15 +1671,12 @@
       <c r="W16" s="4"/>
       <c r="X16" s="2"/>
     </row>
-    <row r="17" spans="1:103" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="2:103" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1000</v>
       </c>
       <c r="AH17" s="3"/>
       <c r="AI17" s="4"/>
@@ -1739,8 +1733,9 @@
       <c r="CH17" s="4"/>
       <c r="CI17" s="2"/>
     </row>
-    <row r="18" spans="1:103" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="2:103" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="AH18" s="6"/>
@@ -1798,15 +1793,12 @@
       <c r="CH18" s="6"/>
       <c r="CI18" s="6"/>
     </row>
-    <row r="19" spans="1:103" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="2:103" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C19" s="1">
-        <v>100000</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="11"/>
@@ -1909,12 +1901,10 @@
       <c r="CX19" s="5"/>
       <c r="CY19" s="11"/>
     </row>
-    <row r="20" spans="1:103" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="2:103" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C20" s="1">
-        <v>20000</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="2"/>
@@ -1950,7 +1940,9 @@
       <c r="CU20" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D14:CY14"/>

</xml_diff>